<commit_message>
Merged changes to port
</commit_message>
<xml_diff>
--- a/houseparts.xlsx
+++ b/houseparts.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28702"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\e-kor\code\SkjellesvikMaterialCost-repo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kathamm\source\repos\SkjellesvikMaterialCost-repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5E84585-0883-4117-9BD3-6FF64866DE55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB56941-9F89-4587-B68E-072D74D61B7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="House parts and materials" sheetId="1" r:id="rId1"/>
+    <sheet name="Materials and suppliers" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>Part</t>
   </si>
@@ -48,12 +49,6 @@
     <t>Metal</t>
   </si>
   <si>
-    <t>Tiles</t>
-  </si>
-  <si>
-    <t>Walls</t>
-  </si>
-  <si>
     <t>Brick</t>
   </si>
   <si>
@@ -69,7 +64,31 @@
     <t>Stone</t>
   </si>
   <si>
-    <t>Pavers</t>
+    <t>External Walls</t>
+  </si>
+  <si>
+    <t>Material</t>
+  </si>
+  <si>
+    <t>Supplier</t>
+  </si>
+  <si>
+    <t>ABC Shingles</t>
+  </si>
+  <si>
+    <t>Cost per unit</t>
+  </si>
+  <si>
+    <t>DEF Shingles</t>
+  </si>
+  <si>
+    <t>ABC Concrete</t>
+  </si>
+  <si>
+    <t>DEF Concrete</t>
+  </si>
+  <si>
+    <t>Glass</t>
   </si>
 </sst>
 </file>
@@ -127,6 +146,21 @@
   </cellStyles>
   <dxfs count="6">
     <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -145,21 +179,6 @@
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -174,15 +193,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{37B2A2DC-BFF6-4B49-BCFE-A008106745B5}" name="MaterialList" displayName="MaterialList" ref="A1:D4" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{37B2A2DC-BFF6-4B49-BCFE-A008106745B5}" name="MaterialList" displayName="MaterialList" ref="A1:D4" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="A1:D4" xr:uid="{37B2A2DC-BFF6-4B49-BCFE-A008106745B5}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{E7D91723-B4CC-4976-9D07-A2F590A004D9}" name="Part" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{9963B7D7-947D-4495-832A-17E810E423F1}" name="Material 1" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{53D1997B-8EAD-4FE1-B8BA-28F08A07D350}" name="Material 2" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{1B3EBE52-7FF1-44C6-A90B-31CF3451CA25}" name="Material 3" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{E7D91723-B4CC-4976-9D07-A2F590A004D9}" name="Part" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{9963B7D7-947D-4495-832A-17E810E423F1}" name="Material 1" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{53D1997B-8EAD-4FE1-B8BA-28F08A07D350}" name="Material 2" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{1B3EBE52-7FF1-44C6-A90B-31CF3451CA25}" name="Material 3" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{42BFEF3C-7567-4D04-8B11-8F10BDA38D92}" name="Table2" displayName="Table2" ref="C3:E7" totalsRowShown="0">
+  <autoFilter ref="C3:E7" xr:uid="{42BFEF3C-7567-4D04-8B11-8F10BDA38D92}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{FF106946-D93E-4743-BC96-653C4C04C030}" name="Material"/>
+    <tableColumn id="2" xr3:uid="{2EAA46E2-C0F4-4284-BEF8-7261A0A87301}" name="Supplier"/>
+    <tableColumn id="3" xr3:uid="{12F36D1F-D6FC-4C00-92D8-C74B7386F469}" name="Cost per unit"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -452,15 +483,16 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="5" width="11.453125" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="11.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -474,7 +506,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -485,35 +517,35 @@
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="2" t="s">
+    </row>
+    <row r="4" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="D4" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -522,4 +554,87 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B76279F-936D-44E0-98BF-539E8E3D1D53}">
+  <dimension ref="C3:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="3" max="3" width="9.33203125" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Standard" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
Added code to update supplier and cost per unit
</commit_message>
<xml_diff>
--- a/houseparts.xlsx
+++ b/houseparts.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kathamm\source\repos\SkjellesvikMaterialCost-repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB56941-9F89-4587-B68E-072D74D61B7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{024F880B-58F6-4A8B-BD03-CA09E036DA87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="House parts and materials" sheetId="1" r:id="rId1"/>
-    <sheet name="Materials and suppliers" sheetId="2" r:id="rId2"/>
+    <sheet name="Supplier and cost" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -206,8 +206,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{42BFEF3C-7567-4D04-8B11-8F10BDA38D92}" name="Table2" displayName="Table2" ref="C3:E7" totalsRowShown="0">
-  <autoFilter ref="C3:E7" xr:uid="{42BFEF3C-7567-4D04-8B11-8F10BDA38D92}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{42BFEF3C-7567-4D04-8B11-8F10BDA38D92}" name="Table2" displayName="Table2" ref="A1:C5" totalsRowShown="0">
+  <autoFilter ref="A1:C5" xr:uid="{42BFEF3C-7567-4D04-8B11-8F10BDA38D92}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{FF106946-D93E-4743-BC96-653C4C04C030}" name="Material"/>
     <tableColumn id="2" xr3:uid="{2EAA46E2-C0F4-4284-BEF8-7261A0A87301}" name="Supplier"/>
@@ -482,7 +482,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -558,70 +558,72 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B76279F-936D-44E0-98BF-539E8E3D1D53}">
-  <dimension ref="C3:E7"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="9.33203125" customWidth="1"/>
+    <col min="1" max="1" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.3984375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:5" x14ac:dyDescent="0.45">
-      <c r="C3" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
         <v>13</v>
       </c>
-      <c r="D3" t="s">
+      <c r="B1" t="s">
         <v>14</v>
       </c>
-      <c r="E3" t="s">
+      <c r="C1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="3:5" x14ac:dyDescent="0.45">
-      <c r="C4" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="D4" t="s">
+      <c r="B2" t="s">
         <v>15</v>
       </c>
-      <c r="E4">
+      <c r="C2">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="3:5" x14ac:dyDescent="0.45">
-      <c r="C5" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="D5" t="s">
+      <c r="B3" t="s">
         <v>17</v>
       </c>
-      <c r="E5">
+      <c r="C3">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="3:5" x14ac:dyDescent="0.45">
-      <c r="C6" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="D6" t="s">
+      <c r="B4" t="s">
         <v>18</v>
       </c>
-      <c r="E6">
+      <c r="C4">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="3:5" x14ac:dyDescent="0.45">
-      <c r="C7" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="D7" t="s">
+      <c r="B5" t="s">
         <v>19</v>
       </c>
-      <c r="E7">
+      <c r="C5">
         <v>34</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update readme and added data for size of parts
</commit_message>
<xml_diff>
--- a/houseparts.xlsx
+++ b/houseparts.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kathamm\source\repos\SkjellesvikMaterialCost-repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{024F880B-58F6-4A8B-BD03-CA09E036DA87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F4FD423-4F28-49A4-B598-EAEE976BA395}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="House parts and materials" sheetId="1" r:id="rId1"/>
-    <sheet name="Supplier and cost" sheetId="2" r:id="rId2"/>
+    <sheet name="House part sizes" sheetId="3" r:id="rId1"/>
+    <sheet name="House parts and materials" sheetId="1" r:id="rId2"/>
+    <sheet name="Supplier and cost" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
   <si>
     <t>Part</t>
   </si>
@@ -89,6 +90,12 @@
   </si>
   <si>
     <t>Glass</t>
+  </si>
+  <si>
+    <t>Square meters</t>
+  </si>
+  <si>
+    <t>External walls</t>
   </si>
 </sst>
 </file>
@@ -193,6 +200,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{096DC52A-7EE2-48B2-97E3-FDC3B64A0517}" name="Table3" displayName="Table3" ref="A1:B4" totalsRowShown="0">
+  <autoFilter ref="A1:B4" xr:uid="{096DC52A-7EE2-48B2-97E3-FDC3B64A0517}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{FF0B5623-ABCE-48EA-A77A-5A2105B6E8DC}" name="Part"/>
+    <tableColumn id="2" xr3:uid="{2712D71D-FF0D-44FD-8D15-371DE30D6DC0}" name="Square meters"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{37B2A2DC-BFF6-4B49-BCFE-A008106745B5}" name="MaterialList" displayName="MaterialList" ref="A1:D4" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="A1:D4" xr:uid="{37B2A2DC-BFF6-4B49-BCFE-A008106745B5}"/>
   <tableColumns count="4">
@@ -205,7 +223,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{42BFEF3C-7567-4D04-8B11-8F10BDA38D92}" name="Table2" displayName="Table2" ref="A1:C5" totalsRowShown="0">
   <autoFilter ref="A1:C5" xr:uid="{42BFEF3C-7567-4D04-8B11-8F10BDA38D92}"/>
   <tableColumns count="3">
@@ -479,6 +497,59 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F86764DF-E9D5-49C0-B088-46FC18066005}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="13.9296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>150</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -556,12 +627,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B76279F-936D-44E0-98BF-539E8E3D1D53}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Updated code to populate the entire table
</commit_message>
<xml_diff>
--- a/houseparts.xlsx
+++ b/houseparts.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kathamm\source\repos\SkjellesvikMaterialCost-repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F4FD423-4F28-49A4-B598-EAEE976BA395}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22FD9B23-C981-4199-8A25-EE3605A187B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="House part sizes" sheetId="3" r:id="rId1"/>
-    <sheet name="House parts and materials" sheetId="1" r:id="rId2"/>
-    <sheet name="Supplier and cost" sheetId="2" r:id="rId3"/>
+    <sheet name="House parts and materials" sheetId="1" r:id="rId1"/>
+    <sheet name="Supplier and cost" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
   <si>
     <t>Part</t>
   </si>
@@ -92,10 +91,7 @@
     <t>Glass</t>
   </si>
   <si>
-    <t>Square meters</t>
-  </si>
-  <si>
-    <t>External walls</t>
+    <t>Size</t>
   </si>
 </sst>
 </file>
@@ -151,7 +147,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -200,30 +199,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{096DC52A-7EE2-48B2-97E3-FDC3B64A0517}" name="Table3" displayName="Table3" ref="A1:B4" totalsRowShown="0">
-  <autoFilter ref="A1:B4" xr:uid="{096DC52A-7EE2-48B2-97E3-FDC3B64A0517}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{FF0B5623-ABCE-48EA-A77A-5A2105B6E8DC}" name="Part"/>
-    <tableColumn id="2" xr3:uid="{2712D71D-FF0D-44FD-8D15-371DE30D6DC0}" name="Square meters"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{37B2A2DC-BFF6-4B49-BCFE-A008106745B5}" name="MaterialList" displayName="MaterialList" ref="A1:D4" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A1:D4" xr:uid="{37B2A2DC-BFF6-4B49-BCFE-A008106745B5}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{E7D91723-B4CC-4976-9D07-A2F590A004D9}" name="Part" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{9963B7D7-947D-4495-832A-17E810E423F1}" name="Material 1" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{53D1997B-8EAD-4FE1-B8BA-28F08A07D350}" name="Material 2" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{1B3EBE52-7FF1-44C6-A90B-31CF3451CA25}" name="Material 3" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{37B2A2DC-BFF6-4B49-BCFE-A008106745B5}" name="MaterialList" displayName="MaterialList" ref="A1:E4" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E4" xr:uid="{37B2A2DC-BFF6-4B49-BCFE-A008106745B5}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{E7D91723-B4CC-4976-9D07-A2F590A004D9}" name="Part" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{9963B7D7-947D-4495-832A-17E810E423F1}" name="Material 1" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{53D1997B-8EAD-4FE1-B8BA-28F08A07D350}" name="Material 2" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{1B3EBE52-7FF1-44C6-A90B-31CF3451CA25}" name="Material 3" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{D103CFA4-74E5-4A19-A042-E15894B7F734}" name="Size" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{42BFEF3C-7567-4D04-8B11-8F10BDA38D92}" name="Table2" displayName="Table2" ref="A1:C5" totalsRowShown="0">
   <autoFilter ref="A1:C5" xr:uid="{42BFEF3C-7567-4D04-8B11-8F10BDA38D92}"/>
   <tableColumns count="3">
@@ -497,64 +486,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F86764DF-E9D5-49C0-B088-46FC18066005}">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="2" max="2" width="13.9296875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4">
-        <v>150</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -563,7 +499,7 @@
     <col min="3" max="5" width="11.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -576,8 +512,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -590,8 +529,11 @@
       <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="E2" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -604,8 +546,11 @@
       <c r="D3" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="E3" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -617,6 +562,9 @@
       </c>
       <c r="D4" s="2" t="s">
         <v>20</v>
+      </c>
+      <c r="E4" s="2">
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -627,7 +575,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B76279F-936D-44E0-98BF-539E8E3D1D53}">
   <dimension ref="A1:C5"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added some more supplier data
</commit_message>
<xml_diff>
--- a/houseparts.xlsx
+++ b/houseparts.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28702"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28703"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kathamm\source\repos\SkjellesvikMaterialCost-repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22FD9B23-C981-4199-8A25-EE3605A187B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A43AF50-0F0B-4E6D-A76E-CD80D0854759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="House parts and materials" sheetId="1" r:id="rId1"/>
     <sheet name="Supplier and cost" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
   <si>
     <t>Part</t>
   </si>
@@ -92,6 +93,18 @@
   </si>
   <si>
     <t>Size</t>
+  </si>
+  <si>
+    <t>Mr Brick</t>
+  </si>
+  <si>
+    <t>The GlassMaster</t>
+  </si>
+  <si>
+    <t>PedalToTheMetal</t>
+  </si>
+  <si>
+    <t>Metallica</t>
   </si>
 </sst>
 </file>
@@ -213,8 +226,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{42BFEF3C-7567-4D04-8B11-8F10BDA38D92}" name="Table2" displayName="Table2" ref="A1:C5" totalsRowShown="0">
-  <autoFilter ref="A1:C5" xr:uid="{42BFEF3C-7567-4D04-8B11-8F10BDA38D92}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{42BFEF3C-7567-4D04-8B11-8F10BDA38D92}" name="Table2" displayName="Table2" ref="A1:C9" totalsRowShown="0">
+  <autoFilter ref="A1:C9" xr:uid="{42BFEF3C-7567-4D04-8B11-8F10BDA38D92}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{FF106946-D93E-4743-BC96-653C4C04C030}" name="Material"/>
     <tableColumn id="2" xr3:uid="{2EAA46E2-C0F4-4284-BEF8-7261A0A87301}" name="Supplier"/>
@@ -489,7 +502,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -577,10 +590,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B76279F-936D-44E0-98BF-539E8E3D1D53}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -646,6 +659,50 @@
         <v>34</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9">
+        <v>76</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>